<commit_message>
Update IP - EX 23 - Formatacao condicional pre-definida (Anexo).xlsx
Exercício
</commit_message>
<xml_diff>
--- a/Materia_2-PowerBi/IP - EX 23 - Formatacao condicional pre-definida (Anexo).xlsx
+++ b/Materia_2-PowerBi/IP - EX 23 - Formatacao condicional pre-definida (Anexo).xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bianc\4)DNC\Repositorio\DNC_DataScience\Materia_2-PowerBi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{813911D8-5BD7-4C52-9DC5-C8A1E5CD2571}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53295EA0-2F02-4984-9DB5-E4B89B4B9632}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19095" yWindow="0" windowWidth="19410" windowHeight="20985" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19095" yWindow="0" windowWidth="19410" windowHeight="20985" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CONTEÚDO" sheetId="1" r:id="rId1"/>
@@ -698,7 +698,275 @@
     <cellStyle name="SAPBEXfilterDrill" xfId="2" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
     <cellStyle name="Vírgula 2" xfId="3" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="27">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
@@ -1406,8 +1674,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B1:Q30"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:Q6"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="M29" sqref="M29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2054,8 +2322,81 @@
     <mergeCell ref="B2:Q6"/>
   </mergeCells>
   <phoneticPr fontId="15" type="noConversion"/>
+  <conditionalFormatting sqref="B11:K19">
+    <cfRule type="colorScale" priority="7">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M10:M18">
+    <cfRule type="cellIs" dxfId="17" priority="6" operator="equal">
+      <formula>"Breno"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B23:C28">
+    <cfRule type="cellIs" dxfId="16" priority="5" operator="greaterThan">
+      <formula>20</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F23:G28">
+    <cfRule type="cellIs" dxfId="15" priority="4" operator="between">
+      <formula>18</formula>
+      <formula>32</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I23:I28">
+    <cfRule type="dataBar" priority="3">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF008AEF"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{6069968B-5F39-4D18-9803-E7E809124A44}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K23:K25">
+    <cfRule type="iconSet" priority="2">
+      <iconSet iconSet="3Symbols">
+        <cfvo type="percent" val="0"/>
+        <cfvo type="percent" val="33"/>
+        <cfvo type="percent" val="67"/>
+      </iconSet>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M23:M30">
+    <cfRule type="aboveAverage" dxfId="11" priority="1"/>
+  </conditionalFormatting>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <drawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
+      <x14:conditionalFormattings>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{6069968B-5F39-4D18-9803-E7E809124A44}">
+            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:borderColor rgb="FF008AEF"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:negativeBorderColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>I23:I28</xm:sqref>
+        </x14:conditionalFormatting>
+      </x14:conditionalFormattings>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -2063,8 +2404,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="B2:I17"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2115,10 +2456,16 @@
       <c r="D4" s="30">
         <v>8</v>
       </c>
-      <c r="E4" s="31"/>
+      <c r="E4" s="31">
+        <f>(C4+(D4*2))/2</f>
+        <v>9.5</v>
+      </c>
       <c r="F4" s="30"/>
       <c r="G4" s="30"/>
-      <c r="H4" s="30"/>
+      <c r="H4" s="30" t="str">
+        <f>IF(E4&gt;=7,"Aprovado",IF(G4&gt;=6,"Aprovado","Reprovado"))</f>
+        <v>Aprovado</v>
+      </c>
       <c r="I4" s="2"/>
     </row>
     <row r="5" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2131,12 +2478,21 @@
       <c r="D5" s="30">
         <v>5</v>
       </c>
-      <c r="E5" s="31"/>
+      <c r="E5" s="31">
+        <f>(C5+(D5*2))/2</f>
+        <v>6</v>
+      </c>
       <c r="F5" s="30">
         <v>6</v>
       </c>
-      <c r="G5" s="30"/>
-      <c r="H5" s="30"/>
+      <c r="G5" s="30">
+        <f>(E5+F5)/2</f>
+        <v>6</v>
+      </c>
+      <c r="H5" s="30" t="str">
+        <f t="shared" ref="H5:H8" si="0">IF(E5&gt;=7,"Aprovado",IF(G5&gt;=6,"Aprovado","Reprovado"))</f>
+        <v>Aprovado</v>
+      </c>
       <c r="I5" s="2"/>
     </row>
     <row r="6" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2149,10 +2505,16 @@
       <c r="D6" s="30">
         <v>6</v>
       </c>
-      <c r="E6" s="31"/>
+      <c r="E6" s="31">
+        <f t="shared" ref="E6:E8" si="1">(C6+(D6*2))/2</f>
+        <v>9</v>
+      </c>
       <c r="F6" s="30"/>
       <c r="G6" s="30"/>
-      <c r="H6" s="30"/>
+      <c r="H6" s="30" t="str">
+        <f t="shared" si="0"/>
+        <v>Aprovado</v>
+      </c>
       <c r="I6" s="2"/>
     </row>
     <row r="7" spans="2:9" x14ac:dyDescent="0.25">
@@ -2165,10 +2527,16 @@
       <c r="D7" s="30">
         <v>7</v>
       </c>
-      <c r="E7" s="31"/>
+      <c r="E7" s="31">
+        <f t="shared" si="1"/>
+        <v>11</v>
+      </c>
       <c r="F7" s="30"/>
       <c r="G7" s="30"/>
-      <c r="H7" s="30"/>
+      <c r="H7" s="30" t="str">
+        <f t="shared" si="0"/>
+        <v>Aprovado</v>
+      </c>
     </row>
     <row r="8" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B8" s="32" t="s">
@@ -2180,12 +2548,21 @@
       <c r="D8" s="30">
         <v>4</v>
       </c>
-      <c r="E8" s="31"/>
+      <c r="E8" s="31">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
       <c r="F8" s="30">
         <v>4</v>
       </c>
-      <c r="G8" s="30"/>
-      <c r="H8" s="30"/>
+      <c r="G8" s="30">
+        <f>(E8+F8)/2</f>
+        <v>4.5</v>
+      </c>
+      <c r="H8" s="30" t="str">
+        <f t="shared" si="0"/>
+        <v>Reprovado</v>
+      </c>
     </row>
     <row r="9" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="10" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
@@ -2253,6 +2630,17 @@
       <c r="E17" s="28"/>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="C4:D8">
+    <cfRule type="cellIs" dxfId="0" priority="4" operator="lessThan">
+      <formula>5</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="3" operator="greaterThan">
+      <formula>5</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
+      <formula>5</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
 </file>
</xml_diff>